<commit_message>
add global & modified button
</commit_message>
<xml_diff>
--- a/新版API.xlsx
+++ b/新版API.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19770" windowHeight="7950" activeTab="1"/>
+    <workbookView windowWidth="19770" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345">
   <si>
     <t>组件名称</t>
   </si>
@@ -171,6 +171,15 @@
     <t>do_Global</t>
   </si>
   <si>
+    <t>http://doc.deviceone.net/web/doc/detail_course/components/do_Global.htm</t>
+  </si>
+  <si>
+    <t>祝钰</t>
+  </si>
+  <si>
+    <t>http://ohtf3vllq.bkt.clouddn.com/do_Global.zip</t>
+  </si>
+  <si>
     <t>do_GridView</t>
   </si>
   <si>
@@ -244,9 +253,6 @@
   </si>
   <si>
     <t>http://doc.deviceone.net/web/doc/detail_course/components/do_PainterView.htm</t>
-  </si>
-  <si>
-    <t>祝钰</t>
   </si>
   <si>
     <t>http://ohtf3vllq.bkt.clouddn.com/do_PainterView.zip</t>
@@ -1102,11 +1108,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1118,32 +1138,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1164,30 +1160,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1202,7 +1177,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1224,6 +1199,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
@@ -1232,9 +1215,32 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1271,19 +1277,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1295,7 +1307,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1307,55 +1325,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1379,7 +1349,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1397,13 +1379,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1415,37 +1451,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1461,8 +1467,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1515,20 +1523,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1556,6 +1553,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1564,10 +1570,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1576,16 +1582,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1594,115 +1600,115 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2057,10 +2063,10 @@
   <sheetPr/>
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I92" sqref="I92"/>
+      <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2301,505 +2307,516 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:9">
       <c r="A42" s="7" t="s">
         <v>49</v>
       </c>
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" t="s">
+        <v>51</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="7" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="7" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" customFormat="1" spans="1:9">
       <c r="A66" s="7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C66" s="9"/>
       <c r="F66" s="9"/>
       <c r="G66" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C87" s="9"/>
       <c r="F87" s="9"/>
       <c r="G87" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="I87" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B92" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C92" s="9"/>
       <c r="F92" s="9"/>
       <c r="G92" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="I92" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="7" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G104" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="G104" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="7" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" s="7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" s="7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" s="7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2809,6 +2826,7 @@
     <hyperlink ref="B66" r:id="rId3" display="http://doc.deviceone.net/web/doc/detail_course/components/do_PainterView.htm"/>
     <hyperlink ref="I66" r:id="rId4" display="http://ohtf3vllq.bkt.clouddn.com/do_PainterView.zip"/>
     <hyperlink ref="I92" r:id="rId5" display="http://ohtf3vllq.bkt.clouddn.com/do_Timer.zip" tooltip="http://ohtf3vllq.bkt.clouddn.com/do_Timer.zip"/>
+    <hyperlink ref="I42" r:id="rId6" display="http://ohtf3vllq.bkt.clouddn.com/do_Global.zip" tooltip="http://ohtf3vllq.bkt.clouddn.com/do_Global.zip"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -2820,7 +2838,7 @@
   <sheetPr/>
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
@@ -2838,25 +2856,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2867,16 +2885,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2887,16 +2905,16 @@
         <v>1.2</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2907,19 +2925,19 @@
         <v>1.2</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2930,19 +2948,19 @@
         <v>3.3</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2953,16 +2971,16 @@
         <v>2.1</v>
       </c>
       <c r="C6" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2973,16 +2991,16 @@
         <v>1.6</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2993,16 +3011,16 @@
         <v>1.1</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -3013,19 +3031,19 @@
         <v>1.3</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F9" t="s">
         <v>149</v>
       </c>
-      <c r="F9" t="s">
-        <v>147</v>
-      </c>
       <c r="G9" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3036,19 +3054,19 @@
         <v>2.1</v>
       </c>
       <c r="C10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" t="s">
         <v>161</v>
       </c>
-      <c r="D10" t="s">
-        <v>159</v>
-      </c>
       <c r="E10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10" t="s">
         <v>149</v>
       </c>
-      <c r="F10" t="s">
-        <v>147</v>
-      </c>
       <c r="G10" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -3059,19 +3077,19 @@
         <v>1.3</v>
       </c>
       <c r="C11" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G11" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3082,16 +3100,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D12" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E12" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3102,19 +3120,19 @@
         <v>1.3</v>
       </c>
       <c r="C13" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -3125,19 +3143,19 @@
         <v>1.8</v>
       </c>
       <c r="C14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -3148,19 +3166,19 @@
         <v>3.3</v>
       </c>
       <c r="C15" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D15" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E15" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G15" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -3171,19 +3189,19 @@
         <v>2.3</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D16" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E16" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3194,16 +3212,16 @@
         <v>1.2</v>
       </c>
       <c r="C17" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E17" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -3214,19 +3232,19 @@
         <v>1.2</v>
       </c>
       <c r="C18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18" t="s">
+        <v>153</v>
+      </c>
+      <c r="E18" t="s">
+        <v>159</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G18" t="s">
         <v>175</v>
-      </c>
-      <c r="D18" t="s">
-        <v>151</v>
-      </c>
-      <c r="E18" t="s">
-        <v>157</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G18" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -3237,19 +3255,19 @@
         <v>2.3</v>
       </c>
       <c r="C19" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E19" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -3260,19 +3278,19 @@
         <v>2.7</v>
       </c>
       <c r="C20" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E20" t="s">
+        <v>151</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G20" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3283,19 +3301,19 @@
         <v>1.6</v>
       </c>
       <c r="C21" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D21" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E21" t="s">
+        <v>151</v>
+      </c>
+      <c r="F21" t="s">
         <v>149</v>
       </c>
-      <c r="F21" t="s">
-        <v>147</v>
-      </c>
       <c r="G21" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -3306,19 +3324,19 @@
         <v>1.1</v>
       </c>
       <c r="C22" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D22" t="s">
+        <v>161</v>
+      </c>
+      <c r="E22" t="s">
         <v>159</v>
       </c>
-      <c r="E22" t="s">
-        <v>157</v>
-      </c>
       <c r="F22" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3329,16 +3347,16 @@
         <v>1.4</v>
       </c>
       <c r="C23" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D23" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E23" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -3349,19 +3367,19 @@
         <v>2.8</v>
       </c>
       <c r="C24" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D24" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E24" t="s">
+        <v>151</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G24" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3372,16 +3390,16 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D25" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E25" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -3392,19 +3410,19 @@
         <v>1.1</v>
       </c>
       <c r="C26" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D26" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E26" t="s">
+        <v>151</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G26" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -3415,19 +3433,19 @@
         <v>2.7</v>
       </c>
       <c r="C27" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D27" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E27" t="s">
+        <v>151</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G27" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -3438,19 +3456,19 @@
         <v>1.7</v>
       </c>
       <c r="C28" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D28" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E28" t="s">
+        <v>151</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G28" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -3461,19 +3479,19 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D29" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E29" t="s">
+        <v>151</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G29" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -3484,19 +3502,19 @@
         <v>1.4</v>
       </c>
       <c r="C30" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D30" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E30" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G30" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3507,16 +3525,16 @@
         <v>1.8</v>
       </c>
       <c r="C31" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D31" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E31" t="s">
+        <v>151</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -3527,19 +3545,19 @@
         <v>2.3</v>
       </c>
       <c r="C32" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D32" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E32" t="s">
+        <v>151</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G32" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -3550,16 +3568,16 @@
         <v>2.4</v>
       </c>
       <c r="C33" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D33" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E33" t="s">
+        <v>151</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -3570,19 +3588,19 @@
         <v>3.9</v>
       </c>
       <c r="C34" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D34" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E34" t="s">
+        <v>151</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G34" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -3593,19 +3611,19 @@
         <v>2.1</v>
       </c>
       <c r="C35" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D35" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E35" t="s">
+        <v>151</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G35" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -3616,19 +3634,19 @@
         <v>1.4</v>
       </c>
       <c r="C36" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E36" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G36" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -3639,19 +3657,19 @@
         <v>2.8</v>
       </c>
       <c r="C37" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D37" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E37" t="s">
+        <v>151</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G37" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -3662,19 +3680,19 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D38" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E38" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G38" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -3685,19 +3703,19 @@
         <v>2.1</v>
       </c>
       <c r="C39" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D39" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E39" t="s">
+        <v>151</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G39" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -3708,19 +3726,19 @@
         <v>2.1</v>
       </c>
       <c r="C40" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D40" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E40" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G40" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -3731,19 +3749,19 @@
         <v>1.6</v>
       </c>
       <c r="C41" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D41" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E41" t="s">
+        <v>151</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G41" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -3754,1750 +3772,1750 @@
         <v>1.4</v>
       </c>
       <c r="C42" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D42" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E42" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B43">
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D43" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E43" t="s">
+        <v>151</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G43" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D44" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E44" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B45">
         <v>1.9</v>
       </c>
       <c r="C45" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D45" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E45" t="s">
+        <v>151</v>
+      </c>
+      <c r="F45" t="s">
         <v>149</v>
       </c>
-      <c r="F45" t="s">
-        <v>147</v>
-      </c>
       <c r="G45" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B46">
         <v>5.4</v>
       </c>
       <c r="C46" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D46" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E46" t="s">
+        <v>151</v>
+      </c>
+      <c r="F46" t="s">
         <v>149</v>
       </c>
-      <c r="F46" t="s">
-        <v>147</v>
-      </c>
       <c r="G46" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B47">
         <v>3.3</v>
       </c>
       <c r="C47" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D47" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E47" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B48">
         <v>1.3</v>
       </c>
       <c r="C48" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D48" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E48" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G48" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B49">
         <v>3.5</v>
       </c>
       <c r="C49" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D49" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E49" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G49" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B50">
         <v>1.4</v>
       </c>
       <c r="C50" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D50" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E50" t="s">
+        <v>151</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B51">
         <v>1.3</v>
       </c>
       <c r="C51" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D51" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E51" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B52">
         <v>4.6</v>
       </c>
       <c r="C52" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D52" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E52" t="s">
+        <v>151</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G52" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B53">
         <v>2.3</v>
       </c>
       <c r="C53" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D53" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E53" t="s">
+        <v>151</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G53" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B54">
         <v>1.1</v>
       </c>
       <c r="C54" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D54" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E54" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B55">
         <v>1.5</v>
       </c>
       <c r="C55" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D55" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E55" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B56">
         <v>3.4</v>
       </c>
       <c r="C56" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D56" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E56" t="s">
+        <v>151</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G56" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B57">
         <v>1.3</v>
       </c>
       <c r="C57" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D57" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E57" t="s">
+        <v>151</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G57" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B58">
         <v>2.2</v>
       </c>
       <c r="C58" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D58" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E58" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G58" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B59">
         <v>6.4</v>
       </c>
       <c r="C59" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D59" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E59" t="s">
+        <v>151</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G59" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B60">
         <v>1.5</v>
       </c>
       <c r="C60" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D60" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E60" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B61">
         <v>1.4</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D61" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E61" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B62">
         <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D62" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E62" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B63">
         <v>2.4</v>
       </c>
       <c r="C63" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D63" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E63" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B64">
         <v>3.2</v>
       </c>
       <c r="C64" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D64" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E64" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B65">
         <v>1.3</v>
       </c>
       <c r="C65" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D65" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E65" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B66">
         <v>1.1</v>
       </c>
       <c r="C66" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D66" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E66" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G66" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B67">
         <v>1.3</v>
       </c>
       <c r="C67" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D67" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E67" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B68">
         <v>1.8</v>
       </c>
       <c r="C68" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D68" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E68" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G68" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B69">
         <v>1.5</v>
       </c>
       <c r="C69" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D69" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E69" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B70">
         <v>1.9</v>
       </c>
       <c r="C70" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D70" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E70" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B71">
         <v>1.1</v>
       </c>
       <c r="C71" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D71" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E71" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G71" s="5"/>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B72">
         <v>1.7</v>
       </c>
       <c r="C72" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D72" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E72" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G72" s="5"/>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B73">
         <v>1.4</v>
       </c>
       <c r="C73" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D73" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E73" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B74">
         <v>1.7</v>
       </c>
       <c r="C74" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D74" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E74" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G74" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B75">
         <v>1.4</v>
       </c>
       <c r="C75" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D75" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E75" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B76">
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D76" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E76" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B77">
         <v>4.8</v>
       </c>
       <c r="C77" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D77" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E77" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G77" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B78">
         <v>1.2</v>
       </c>
       <c r="C78" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D78" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E78" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B79">
         <v>2.9</v>
       </c>
       <c r="C79" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D79" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E79" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G79" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B80">
         <v>1.1</v>
       </c>
       <c r="C80" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D80" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E80" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B81">
         <v>2.4</v>
       </c>
       <c r="C81" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D81" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E81" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B82">
         <v>2.8</v>
       </c>
       <c r="C82" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D82" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E82" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B83">
         <v>5.5</v>
       </c>
       <c r="C83" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D83" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E83" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B84">
         <v>2</v>
       </c>
       <c r="C84" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D84" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E84" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G84" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B85">
         <v>2.9</v>
       </c>
       <c r="C85" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D85" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E85" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B86">
         <v>1.6</v>
       </c>
       <c r="C86" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D86" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E86" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G86" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B87">
         <v>2.2</v>
       </c>
       <c r="C87" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D87" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E87" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B88">
         <v>2.7</v>
       </c>
       <c r="C88" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D88" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E88" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B89">
         <v>2.6</v>
       </c>
       <c r="C89" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D89" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E89" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B90">
         <v>5.7</v>
       </c>
       <c r="C90" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D90" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E90" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B91">
         <v>5.7</v>
       </c>
       <c r="C91" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D91" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E91" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B92">
         <v>2.3</v>
       </c>
       <c r="C92" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D92" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E92" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B93">
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D93" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E93" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B94">
         <v>1.4</v>
       </c>
       <c r="C94" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D94" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E94" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B95">
         <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D95" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E95" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B96">
         <v>1.4</v>
       </c>
       <c r="C96" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D96" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E96" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B97">
         <v>1.4</v>
       </c>
       <c r="C97" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D97" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E97" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B98">
         <v>1.8</v>
       </c>
       <c r="C98" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D98" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E98" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B99">
         <v>2.1</v>
       </c>
       <c r="C99" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D99" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E99" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B100">
         <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D100" t="s">
+        <v>161</v>
+      </c>
+      <c r="E100" t="s">
         <v>159</v>
       </c>
-      <c r="E100" t="s">
-        <v>157</v>
-      </c>
       <c r="F100" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B101">
         <v>2.4</v>
       </c>
       <c r="C101" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D101" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E101" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="G101" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B102">
         <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D102" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E102" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B103">
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D103" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E103" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G103" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B104">
         <v>1.1</v>
       </c>
       <c r="C104" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D104" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E104" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B105">
         <v>1</v>
       </c>
       <c r="C105" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D105" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E105" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G105" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B106">
         <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D106" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E106" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B107">
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D107" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E107" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B108">
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D108" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E108" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B109">
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D109" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E109" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B110">
         <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D110" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E110" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B111">
         <v>1.1</v>
       </c>
       <c r="C111" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D111" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E111" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B112">
         <v>1.3</v>
       </c>
       <c r="C112" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D112" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E112" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B113">
         <v>1</v>
       </c>
       <c r="C113" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D113" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E113" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B114">
         <v>1.1</v>
       </c>
       <c r="C114" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D114" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E114" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B115">
         <v>1</v>
       </c>
       <c r="C115" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D115" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E115" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B116">
         <v>1.1</v>
       </c>
       <c r="C116" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D116" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E116" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B117">
         <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D117" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E117" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B118">
         <v>1</v>
       </c>
       <c r="C118" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D118" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E118" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B119">
         <v>1.2</v>
       </c>
       <c r="C119" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D119" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E119" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B120">
         <v>1.2</v>
       </c>
       <c r="C120" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D120" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E120" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B121">
         <v>1.1</v>
       </c>
       <c r="C121" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D121" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E121" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B122">
         <v>2.1</v>
       </c>
       <c r="C122" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D122" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E122" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -5574,7 +5592,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -5582,18 +5600,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>